<commit_message>
Trying second approach: copy and pasting data instead of scraping.
</commit_message>
<xml_diff>
--- a/tree.xlsx
+++ b/tree.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herman/Documents/kaGrader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7B969361-01A7-6A42-8AAB-29B4F3A4034A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151F44BB-2516-7648-ACD4-85BADDE650CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="21520"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tree" sheetId="1" r:id="rId1"/>
+    <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tree!$A$1:$E$207</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="221">
   <si>
     <t>Analyzing categorical data</t>
   </si>
@@ -596,37 +600,109 @@
     <t>Transformations to achieve linearity</t>
   </si>
   <si>
-    <t>Prepare for the 2019 AP¬ÆÔ∏é Statistics Exam</t>
-  </si>
-  <si>
     <t>Prepare for the exam</t>
   </si>
   <si>
     <t>Choosing an appropriate inference procedure</t>
   </si>
   <si>
-    <t>AP¬ÆÔ∏é Statistics Standards mappings</t>
-  </si>
-  <si>
-    <t>See how our course content aligns with AP¬ÆÔ∏é Statistics Standards</t>
-  </si>
-  <si>
     <t>Book Section</t>
   </si>
   <si>
-    <t>§2.5</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>…</t>
+    <t>nic</t>
+  </si>
+  <si>
+    <t>AP® Statistics Standards mappings</t>
+  </si>
+  <si>
+    <t>See how our course content aligns with AP® Statistics Standards</t>
+  </si>
+  <si>
+    <t>Book section legend</t>
+  </si>
+  <si>
+    <t>nic = not in curriculum, so I haven't mapped to book section</t>
+  </si>
+  <si>
+    <t>Writing hypotheses for testing the difference of means</t>
+  </si>
+  <si>
+    <t>Test statistic in a two-sample t test</t>
+  </si>
+  <si>
+    <t>P-value in a two-sample t test</t>
+  </si>
+  <si>
+    <t>Making conclusions about the difference of means</t>
+  </si>
+  <si>
+    <t>Conditions for inference on two means</t>
+  </si>
+  <si>
+    <t>Two-sample t interval for the difference of means</t>
+  </si>
+  <si>
+    <t>Prepare for the 2019 AP® Statistics Exam</t>
+  </si>
+  <si>
+    <t>Create histograms</t>
+  </si>
+  <si>
+    <t>Read histograms</t>
+  </si>
+  <si>
+    <t>Reading stem and leaf plots</t>
+  </si>
+  <si>
+    <t>1.3,1.4</t>
+  </si>
+  <si>
+    <t>2.1-2.3</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>4.1-4.3</t>
+  </si>
+  <si>
+    <t>4.4-4.5</t>
+  </si>
+  <si>
+    <t>? = in curriculum, but I haven't mapped</t>
+  </si>
+  <si>
+    <t>7.2,8.2</t>
+  </si>
+  <si>
+    <t>6.3,6.5,8.1</t>
+  </si>
+  <si>
+    <t>7.1,8.1</t>
+  </si>
+  <si>
+    <t>5.3,6.1</t>
+  </si>
+  <si>
+    <t>OriginalOrder</t>
+  </si>
+  <si>
+    <t>1.1,2.5</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Lesson</t>
+  </si>
+  <si>
+    <t>Exercise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="12"/>
@@ -1480,1342 +1556,2351 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D197"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" hidden="1">
       <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:5" hidden="1">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="2" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1">
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="C6" t="s">
+    <row r="6" spans="1:5">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4.3</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E8">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E9">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="C11" t="s">
+    <row r="11" spans="1:5">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E11">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E12">
         <v>11</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" t="s">
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E13">
         <v>12</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:5" hidden="1">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="C16" t="s">
+    <row r="16" spans="1:5" hidden="1">
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E16">
         <v>15</v>
       </c>
-      <c r="D16">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="C17" t="s">
-        <v>16</v>
+    </row>
+    <row r="17" spans="1:5" hidden="1">
+      <c r="C17" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D17">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="B18" s="2" t="s">
+      <c r="E17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1">
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>1.2</v>
+      </c>
+      <c r="E18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5" hidden="1">
       <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="C20" t="s">
+    <row r="20" spans="1:5" hidden="1">
+      <c r="C20" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E20">
         <v>19</v>
       </c>
-      <c r="D20">
+    </row>
+    <row r="21" spans="1:5" hidden="1">
+      <c r="C21" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="C21" t="s">
+      <c r="E21">
         <v>20</v>
       </c>
-      <c r="D21">
+    </row>
+    <row r="22" spans="1:5" hidden="1">
+      <c r="C22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="C22" t="s">
+      <c r="E22">
         <v>21</v>
       </c>
-      <c r="D22">
+    </row>
+    <row r="23" spans="1:5" hidden="1">
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="E23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="1:5" hidden="1">
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>1.2</v>
+      </c>
+      <c r="E24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="C25" t="s">
+    <row r="25" spans="1:5" hidden="1">
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>1.2</v>
+      </c>
+      <c r="E25">
         <v>24</v>
       </c>
-      <c r="D25">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="C26" t="s">
+    </row>
+    <row r="26" spans="1:5" hidden="1">
+      <c r="C26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>1.2</v>
+      </c>
+      <c r="E26">
         <v>25</v>
       </c>
-      <c r="D26">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="C27" t="s">
-        <v>26</v>
+    </row>
+    <row r="27" spans="1:5" hidden="1">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D27">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1">
       <c r="B28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>1.3</v>
+      </c>
+      <c r="E28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="C29" t="s">
-        <v>28</v>
+    <row r="29" spans="1:5" hidden="1">
+      <c r="C29" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D29">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="C30" t="s">
-        <v>29</v>
+      <c r="E29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1">
+      <c r="C30" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D30">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="C31" t="s">
-        <v>30</v>
+      <c r="E30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1">
+      <c r="C31" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D31">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1">
       <c r="B32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32">
+        <v>1.3</v>
+      </c>
+      <c r="E32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="C33" t="s">
-        <v>32</v>
+    <row r="33" spans="1:5" hidden="1">
+      <c r="C33" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D33">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="C34" t="s">
-        <v>33</v>
+      <c r="E33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1">
+      <c r="C34" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D34">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="C35" t="s">
-        <v>34</v>
+      <c r="E34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1">
+      <c r="C35" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D35">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" hidden="1">
       <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36">
+        <v>1.3</v>
+      </c>
+      <c r="E36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="B37" s="2" t="s">
+    <row r="37" spans="1:5" hidden="1">
+      <c r="C37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>1.3</v>
+      </c>
+      <c r="E37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="C38" t="s">
-        <v>37</v>
+    <row r="38" spans="1:5" hidden="1">
+      <c r="C38" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D38">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="C39" t="s">
-        <v>38</v>
+      <c r="E38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1">
+      <c r="C39" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D39">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="C40" t="s">
-        <v>39</v>
+      <c r="E39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1">
+      <c r="B40" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D40">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="C41" t="s">
-        <v>40</v>
+      <c r="E40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1">
+      <c r="B41" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D41">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
+      <c r="E41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1">
+      <c r="C42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42">
+        <v>1.3</v>
+      </c>
+      <c r="E42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="B43" s="2" t="s">
+    <row r="43" spans="1:5" hidden="1">
+      <c r="C43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43">
+        <v>1.3</v>
+      </c>
+      <c r="E43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="C44" t="s">
-        <v>43</v>
+    <row r="44" spans="1:5" hidden="1">
+      <c r="C44" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D44">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="B45" s="2" t="s">
+      <c r="E44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1">
+      <c r="C45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>1.3</v>
+      </c>
+      <c r="E45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="C46" t="s">
-        <v>45</v>
+    <row r="46" spans="1:5" hidden="1">
+      <c r="A46" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D46">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="C47" t="s">
+      <c r="E46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1">
+      <c r="B47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" t="s">
+        <v>206</v>
+      </c>
+      <c r="E47">
         <v>46</v>
       </c>
-      <c r="D47">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="B48" s="2" t="s">
+    </row>
+    <row r="48" spans="1:5" hidden="1">
+      <c r="C48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48">
+        <v>1.3</v>
+      </c>
+      <c r="E48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="C49" t="s">
-        <v>48</v>
+    <row r="49" spans="1:5" hidden="1">
+      <c r="B49" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D49">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="B50" s="2" t="s">
+      <c r="E49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" hidden="1">
+      <c r="C50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50">
+        <v>1.4</v>
+      </c>
+      <c r="E50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="C51" t="s">
-        <v>50</v>
+    <row r="51" spans="1:5" hidden="1">
+      <c r="C51" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D51">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="C52" t="s">
-        <v>51</v>
+      <c r="E51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1">
+      <c r="B52" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D52">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53" s="2" t="s">
+      <c r="E52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1">
+      <c r="C53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53">
+        <v>1.4</v>
+      </c>
+      <c r="E53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="C54" t="s">
-        <v>53</v>
+    <row r="54" spans="1:5" hidden="1">
+      <c r="B54" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D54">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="B55" s="2" t="s">
+      <c r="E54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1">
+      <c r="C55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55">
+        <v>1.4</v>
+      </c>
+      <c r="E55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="C56" t="s">
-        <v>55</v>
+    <row r="56" spans="1:5" hidden="1">
+      <c r="C56" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="D56">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="C57" t="s">
-        <v>56</v>
+      <c r="E56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" hidden="1">
+      <c r="B57" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D57">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="C58" t="s">
-        <v>57</v>
+      <c r="E57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1">
+      <c r="C58" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D58">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
+      <c r="E58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" hidden="1">
+      <c r="B59" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59">
+        <v>1.4</v>
+      </c>
+      <c r="E59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="B60" s="2" t="s">
+    <row r="60" spans="1:5" hidden="1">
+      <c r="C60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60">
+        <v>1.4</v>
+      </c>
+      <c r="E60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="C61" t="s">
+    <row r="61" spans="1:5" hidden="1">
+      <c r="C61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61">
+        <v>1.4</v>
+      </c>
+      <c r="E61">
         <v>60</v>
       </c>
-      <c r="D61">
+    </row>
+    <row r="62" spans="1:5" hidden="1">
+      <c r="C62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62">
+        <v>1.4</v>
+      </c>
+      <c r="E62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" hidden="1">
+      <c r="A63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" t="s">
+        <v>207</v>
+      </c>
+      <c r="E63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" hidden="1">
+      <c r="B64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="C62" t="s">
+      <c r="E64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" hidden="1">
+      <c r="C65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65">
+        <v>2.1</v>
+      </c>
+      <c r="E65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" hidden="1">
+      <c r="C66" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D62">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="C63" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="C64" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="B65" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="C66" t="s">
-        <v>65</v>
       </c>
       <c r="D66">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="B67" s="2" t="s">
+      <c r="E66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1">
+      <c r="C67" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="C68" t="s">
+    <row r="68" spans="1:5" hidden="1">
+      <c r="C68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E68">
         <v>67</v>
       </c>
-      <c r="D68">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="C69" t="s">
+    </row>
+    <row r="69" spans="1:5" hidden="1">
+      <c r="B69" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E69">
         <v>68</v>
       </c>
-      <c r="D69">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="C70" t="s">
+    </row>
+    <row r="70" spans="1:5" hidden="1">
+      <c r="C70" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E70">
         <v>69</v>
       </c>
-      <c r="D70">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="C71" t="s">
-        <v>70</v>
+    </row>
+    <row r="71" spans="1:5" hidden="1">
+      <c r="B71" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D71">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="B72" s="2" t="s">
+      <c r="E71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" hidden="1">
+      <c r="C72" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="C73" t="s">
-        <v>72</v>
+    <row r="73" spans="1:5" hidden="1">
+      <c r="C73" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D73">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="C74" t="s">
-        <v>73</v>
+      <c r="E73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1">
+      <c r="C74" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D74">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="1" t="s">
+      <c r="E74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" hidden="1">
+      <c r="C75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5" hidden="1">
       <c r="B76" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="C77" t="s">
+    <row r="77" spans="1:5" hidden="1">
+      <c r="C77" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E77">
         <v>76</v>
       </c>
-      <c r="D77">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="C78" t="s">
+    </row>
+    <row r="78" spans="1:5" hidden="1">
+      <c r="C78" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D78">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E78">
         <v>77</v>
       </c>
-      <c r="D78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="C79" t="s">
-        <v>78</v>
+    </row>
+    <row r="79" spans="1:5" hidden="1">
+      <c r="A79" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D79">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1">
       <c r="B80" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="C81" t="s">
-        <v>80</v>
+    <row r="81" spans="1:5" hidden="1">
+      <c r="C81" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="C82" t="s">
-        <v>79</v>
+      <c r="E81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1">
+      <c r="C82" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="D82">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="B83" s="2" t="s">
+      <c r="E82">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="C84" t="s">
+    <row r="83" spans="1:5" hidden="1">
+      <c r="C83" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83">
         <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" hidden="1">
+      <c r="B84" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D84">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="B85" s="2" t="s">
+      <c r="E84">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="C86" t="s">
+    <row r="85" spans="1:5" hidden="1">
+      <c r="C85" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85">
         <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" hidden="1">
+      <c r="C86" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D86">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="C87" t="s">
+      <c r="E86">
         <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1">
+      <c r="B87" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="C88" t="s">
+      <c r="E87">
         <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" hidden="1">
+      <c r="C88" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="1" t="s">
+      <c r="E88">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="B90" s="2" t="s">
+    <row r="89" spans="1:5" hidden="1">
+      <c r="B89" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="C91" t="s">
+    <row r="90" spans="1:5" hidden="1">
+      <c r="C90" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+      <c r="E90">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
-      <c r="B92" s="2" t="s">
+    <row r="91" spans="1:5" hidden="1">
+      <c r="C91" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="C93" t="s">
+    <row r="92" spans="1:5" hidden="1">
+      <c r="C92" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+      <c r="E92">
         <v>91</v>
       </c>
-      <c r="D93">
+    </row>
+    <row r="93" spans="1:5" hidden="1">
+      <c r="A93" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D93" t="s">
+        <v>209</v>
+      </c>
+      <c r="E93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="B94" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D94">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="C95" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D95" t="s">
+        <v>208</v>
+      </c>
+      <c r="E95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="B96" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D96">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="B94" s="2" t="s">
+      <c r="E96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="C97" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D97">
+        <v>4.2</v>
+      </c>
+      <c r="E97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="B98" s="2" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="C95" t="s">
-        <v>93</v>
-      </c>
-      <c r="D95">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="C96" t="s">
-        <v>94</v>
-      </c>
-      <c r="D96">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="C97" t="s">
-        <v>95</v>
-      </c>
-      <c r="D97">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="C98" t="s">
-        <v>96</v>
       </c>
       <c r="D98">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="B99" s="2" t="s">
+      <c r="E98">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="C100" t="s">
+    <row r="99" spans="1:5">
+      <c r="C99" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D99">
+        <v>4.3</v>
+      </c>
+      <c r="E99">
         <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="C100" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D100">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1" t="s">
+      <c r="E100">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="B102" s="2" t="s">
+    <row r="101" spans="1:5">
+      <c r="C101" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D101">
+        <v>4.3</v>
+      </c>
+      <c r="E101">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="C103" t="s">
+    <row r="102" spans="1:5">
+      <c r="C102" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D102">
+        <v>4.3</v>
+      </c>
+      <c r="E102">
         <v>101</v>
       </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="B103" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D103">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="C104" t="s">
+        <v>4.3</v>
+      </c>
+      <c r="E103">
         <v>102</v>
       </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="C104" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D104">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="C105" t="s">
+        <v>4.3</v>
+      </c>
+      <c r="E104">
         <v>103</v>
       </c>
-      <c r="D105">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+    </row>
+    <row r="105" spans="1:5" hidden="1">
+      <c r="A105" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D105" t="s">
+        <v>210</v>
+      </c>
+      <c r="E105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" hidden="1">
       <c r="B106" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="C107" t="s">
+        <v>100</v>
+      </c>
+      <c r="D106" t="s">
+        <v>210</v>
+      </c>
+      <c r="E106">
         <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" hidden="1">
+      <c r="C107" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="D107">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="C108" t="s">
+      <c r="E107">
         <v>106</v>
       </c>
+    </row>
+    <row r="108" spans="1:5" hidden="1">
+      <c r="C108" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D108">
+        <v>4.5</v>
+      </c>
+      <c r="E108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" hidden="1">
+      <c r="C109" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D109">
+        <v>4.5</v>
+      </c>
+      <c r="E109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" hidden="1">
+      <c r="B110" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D110">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="B109" s="2" t="s">
+      <c r="E110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" hidden="1">
+      <c r="C111" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D111">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" hidden="1">
+      <c r="C112" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D112">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="B113" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="C110" t="s">
+      <c r="D113" t="s">
+        <v>208</v>
+      </c>
+      <c r="E113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="C114" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D110" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="B111" s="2" t="s">
+      <c r="D114" t="s">
+        <v>208</v>
+      </c>
+      <c r="E114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="B115" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="C112" t="s">
+      <c r="D115" t="s">
+        <v>208</v>
+      </c>
+      <c r="E115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" hidden="1">
+      <c r="C116" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D112">
+      <c r="D116">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="C113" t="s">
+      <c r="E116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" hidden="1">
+      <c r="C117" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D113">
+      <c r="D117">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="B114" s="2" t="s">
+      <c r="E117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" hidden="1">
+      <c r="B118" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="C115" t="s">
+      <c r="D118">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" hidden="1">
+      <c r="C119" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D115">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="C116" t="s">
-        <v>112</v>
-      </c>
-      <c r="D116">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="C117" t="s">
-        <v>113</v>
-      </c>
-      <c r="D117">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="B118" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="C119" t="s">
-        <v>115</v>
       </c>
       <c r="D119">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="B120" s="2" t="s">
+      <c r="E119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" hidden="1">
+      <c r="C120" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D120">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" hidden="1">
+      <c r="C121" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D121">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" hidden="1">
+      <c r="B122" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D122">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" hidden="1">
+      <c r="C123" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D123">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" hidden="1">
+      <c r="B124" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="C121" t="s">
+      <c r="D124" t="s">
+        <v>191</v>
+      </c>
+      <c r="E124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" hidden="1">
+      <c r="C125" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D121" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="C122" t="s">
+      <c r="D125" t="s">
+        <v>191</v>
+      </c>
+      <c r="E125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" hidden="1">
+      <c r="C126" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D122" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="C123" t="s">
+      <c r="D126" t="s">
+        <v>191</v>
+      </c>
+      <c r="E126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" hidden="1">
+      <c r="C127" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D123" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="1" t="s">
+      <c r="D127" t="s">
+        <v>191</v>
+      </c>
+      <c r="E127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" hidden="1">
+      <c r="A128" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="B125" s="2" t="s">
+      <c r="D128" t="s">
+        <v>215</v>
+      </c>
+      <c r="E128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" hidden="1">
+      <c r="B129" s="2" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="C126" t="s">
-        <v>122</v>
-      </c>
-      <c r="D126">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="B127" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
-      <c r="C128" t="s">
-        <v>124</v>
-      </c>
-      <c r="D128">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
-      <c r="C129" t="s">
-        <v>125</v>
       </c>
       <c r="D129">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="C130" t="s">
-        <v>126</v>
+      <c r="E129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" hidden="1">
+      <c r="C130" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="D130">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" hidden="1">
       <c r="B131" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D131">
+        <v>5.3</v>
+      </c>
+      <c r="E131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" hidden="1">
+      <c r="C132" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D132">
+        <v>5.3</v>
+      </c>
+      <c r="E132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" hidden="1">
+      <c r="C133" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D133">
+        <v>5.3</v>
+      </c>
+      <c r="E133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" hidden="1">
+      <c r="C134" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D134">
+        <v>5.3</v>
+      </c>
+      <c r="E134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" hidden="1">
+      <c r="B135" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="C132" t="s">
+      <c r="D135">
+        <v>6.1</v>
+      </c>
+      <c r="E135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" hidden="1">
+      <c r="C136" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D132">
+      <c r="D136">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="C133" t="s">
+      <c r="E136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" hidden="1">
+      <c r="C137" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D133">
+      <c r="D137">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="C134" t="s">
+      <c r="E137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" hidden="1">
+      <c r="C138" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D134">
+      <c r="D138">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="1" t="s">
+      <c r="E138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" hidden="1">
+      <c r="A139" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="B136" s="2" t="s">
+      <c r="D139" t="s">
+        <v>214</v>
+      </c>
+      <c r="E139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="B140" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="B137" s="2" t="s">
+      <c r="D140" t="s">
+        <v>208</v>
+      </c>
+      <c r="E140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" hidden="1">
+      <c r="B141" s="2" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="C138" t="s">
-        <v>134</v>
-      </c>
-      <c r="D138">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="C139" t="s">
-        <v>135</v>
-      </c>
-      <c r="D139">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="C140" t="s">
-        <v>136</v>
-      </c>
-      <c r="D140">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="C141" t="s">
-        <v>137</v>
       </c>
       <c r="D141">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="B142" s="2" t="s">
+      <c r="E141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" hidden="1">
+      <c r="C142" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D142">
+        <v>8.1</v>
+      </c>
+      <c r="E142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" hidden="1">
+      <c r="C143" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D143">
+        <v>8.1</v>
+      </c>
+      <c r="E143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" hidden="1">
+      <c r="C144" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D144">
+        <v>8.1</v>
+      </c>
+      <c r="E144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" hidden="1">
+      <c r="C145" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D145">
+        <v>8.1</v>
+      </c>
+      <c r="E145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" hidden="1">
+      <c r="B146" s="2" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="C143" t="s">
-        <v>139</v>
-      </c>
-      <c r="D143">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="C144" t="s">
-        <v>140</v>
-      </c>
-      <c r="D144">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
-      <c r="C145" t="s">
-        <v>141</v>
-      </c>
-      <c r="D145">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="C146" t="s">
-        <v>142</v>
       </c>
       <c r="D146">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
-      <c r="A147" s="1" t="s">
+      <c r="E146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" hidden="1">
+      <c r="C147" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D147">
+        <v>7.1</v>
+      </c>
+      <c r="E147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" hidden="1">
+      <c r="C148" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D148">
+        <v>7.1</v>
+      </c>
+      <c r="E148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" hidden="1">
+      <c r="C149" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D149">
+        <v>7.1</v>
+      </c>
+      <c r="E149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" hidden="1">
+      <c r="C150" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D150">
+        <v>7.1</v>
+      </c>
+      <c r="E150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" hidden="1">
+      <c r="A151" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="B148" s="2" t="s">
+      <c r="D151" t="s">
+        <v>213</v>
+      </c>
+      <c r="E151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" hidden="1">
+      <c r="B152" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="C149" t="s">
+      <c r="D152">
+        <v>6.3</v>
+      </c>
+      <c r="E152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" hidden="1">
+      <c r="C153" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D149">
+      <c r="D153">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="C150" t="s">
+      <c r="E153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" hidden="1">
+      <c r="C154" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D150">
+      <c r="D154">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="B151" s="2" t="s">
+      <c r="E154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" hidden="1">
+      <c r="B155" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="C152" t="s">
+      <c r="D155">
+        <v>6.5</v>
+      </c>
+      <c r="E155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" hidden="1">
+      <c r="C156" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D152">
+      <c r="D156">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="C153" t="s">
+      <c r="E156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" hidden="1">
+      <c r="C157" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D153">
+      <c r="D157">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="B154" s="2" t="s">
+      <c r="E157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" hidden="1">
+      <c r="B158" s="2" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="C155" t="s">
-        <v>150</v>
-      </c>
-      <c r="D155">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="C156" t="s">
-        <v>151</v>
-      </c>
-      <c r="D156">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="C157" t="s">
-        <v>152</v>
-      </c>
-      <c r="D157">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="C158" t="s">
-        <v>153</v>
       </c>
       <c r="D158">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="C159" t="s">
-        <v>154</v>
+      <c r="E158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" hidden="1">
+      <c r="C159" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="D159">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="B160" s="2" t="s">
+      <c r="E159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" hidden="1">
+      <c r="C160" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D160">
+        <v>8.1</v>
+      </c>
+      <c r="E160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" hidden="1">
+      <c r="C161" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D161">
+        <v>8.1</v>
+      </c>
+      <c r="E161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" hidden="1">
+      <c r="C162" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D162">
+        <v>8.1</v>
+      </c>
+      <c r="E162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" hidden="1">
+      <c r="C163" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D163">
+        <v>8.1</v>
+      </c>
+      <c r="E163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" hidden="1">
+      <c r="B164" s="2" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
-      <c r="C161" t="s">
-        <v>156</v>
-      </c>
-      <c r="D161">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
-      <c r="C162" t="s">
-        <v>157</v>
-      </c>
-      <c r="D162">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
-      <c r="C163" t="s">
-        <v>158</v>
-      </c>
-      <c r="D163">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
-      <c r="C164" t="s">
-        <v>159</v>
       </c>
       <c r="D164">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="165" spans="1:4">
-      <c r="C165" t="s">
-        <v>160</v>
+      <c r="E164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" hidden="1">
+      <c r="C165" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="D165">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
-      <c r="A166" s="1" t="s">
+      <c r="E165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" hidden="1">
+      <c r="C166" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D166">
+        <v>6.3</v>
+      </c>
+      <c r="E166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" hidden="1">
+      <c r="C167" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D167">
+        <v>6.3</v>
+      </c>
+      <c r="E167">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" hidden="1">
+      <c r="C168" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D168">
+        <v>6.3</v>
+      </c>
+      <c r="E168">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" hidden="1">
+      <c r="C169" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D169">
+        <v>6.3</v>
+      </c>
+      <c r="E169">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" hidden="1">
+      <c r="A170" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="167" spans="1:4">
-      <c r="B167" s="2" t="s">
+      <c r="D170" t="s">
+        <v>212</v>
+      </c>
+      <c r="E170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" hidden="1">
+      <c r="B171" s="2" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
-      <c r="C168" t="s">
-        <v>163</v>
-      </c>
-      <c r="D168">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
-      <c r="C169" t="s">
-        <v>164</v>
-      </c>
-      <c r="D169">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
-      <c r="B170" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
-      <c r="C171" t="s">
-        <v>166</v>
       </c>
       <c r="D171">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="172" spans="1:4">
-      <c r="C172" t="s">
+      <c r="E171">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" hidden="1">
+      <c r="C172" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D172">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E172">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" hidden="1">
+      <c r="C173" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D173">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E173">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" hidden="1">
+      <c r="B174" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D174">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E174">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" hidden="1">
+      <c r="C175" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D175">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E175">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" hidden="1">
+      <c r="C176" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="173" spans="1:4">
-      <c r="C173" t="s">
+      <c r="D176">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E176">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" hidden="1">
+      <c r="C177" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="C174" t="s">
+      <c r="D177">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E177">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" hidden="1">
+      <c r="C178" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="175" spans="1:4">
-      <c r="B175" s="2" t="s">
+      <c r="D178">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E178">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" hidden="1">
+      <c r="B179" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D175">
+      <c r="D179">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="176" spans="1:4">
-      <c r="B176" s="2" t="s">
+      <c r="E179">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" hidden="1">
+      <c r="C180" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D180">
+        <v>7.2</v>
+      </c>
+      <c r="E180">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" hidden="1">
+      <c r="C181" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D181">
+        <v>7.2</v>
+      </c>
+      <c r="E181">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" hidden="1">
+      <c r="B182" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D176">
+      <c r="D182">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="A177" s="1" t="s">
+      <c r="E182">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" hidden="1">
+      <c r="C183" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D183">
+        <v>7.2</v>
+      </c>
+      <c r="E183">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" hidden="1">
+      <c r="C184" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D184">
+        <v>7.2</v>
+      </c>
+      <c r="E184">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" hidden="1">
+      <c r="C185" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D185">
+        <v>7.2</v>
+      </c>
+      <c r="E185">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" hidden="1">
+      <c r="C186" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D186">
+        <v>7.2</v>
+      </c>
+      <c r="E186">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" hidden="1">
+      <c r="A187" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="B178" s="2" t="s">
+      <c r="D187" t="s">
+        <v>191</v>
+      </c>
+      <c r="E187">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" hidden="1">
+      <c r="B188" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="C179" t="s">
+      <c r="D188" t="s">
+        <v>191</v>
+      </c>
+      <c r="E188">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" hidden="1">
+      <c r="C189" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="C180" t="s">
+      <c r="D189" t="s">
+        <v>191</v>
+      </c>
+      <c r="E189">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" hidden="1">
+      <c r="C190" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="C181" t="s">
+      <c r="D190" t="s">
+        <v>191</v>
+      </c>
+      <c r="E190">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" hidden="1">
+      <c r="C191" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="C182" t="s">
+      <c r="D191" t="s">
+        <v>191</v>
+      </c>
+      <c r="E191">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" hidden="1">
+      <c r="C192" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="B183" s="2" t="s">
+      <c r="D192" t="s">
+        <v>191</v>
+      </c>
+      <c r="E192">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" hidden="1">
+      <c r="B193" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="C184" t="s">
+      <c r="D193" t="s">
+        <v>191</v>
+      </c>
+      <c r="E193">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" hidden="1">
+      <c r="C194" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="C185" t="s">
+      <c r="D194" t="s">
+        <v>191</v>
+      </c>
+      <c r="E194">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" hidden="1">
+      <c r="C195" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="C186" t="s">
+      <c r="D195" t="s">
+        <v>191</v>
+      </c>
+      <c r="E195">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" hidden="1">
+      <c r="C196" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="1" t="s">
+      <c r="D196" t="s">
+        <v>191</v>
+      </c>
+      <c r="E196">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" hidden="1">
+      <c r="A197" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="B188" s="2" t="s">
+      <c r="D197" t="s">
+        <v>191</v>
+      </c>
+      <c r="E197">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" hidden="1">
+      <c r="B198" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="C189" t="s">
+      <c r="D198" t="s">
+        <v>191</v>
+      </c>
+      <c r="E198">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" hidden="1">
+      <c r="C199" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="C190" t="s">
+      <c r="D199" t="s">
+        <v>191</v>
+      </c>
+      <c r="E199">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" hidden="1">
+      <c r="C200" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="C191" t="s">
+      <c r="D200" t="s">
+        <v>191</v>
+      </c>
+      <c r="E200">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" hidden="1">
+      <c r="C201" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="B192" s="2" t="s">
+      <c r="D201" t="s">
+        <v>191</v>
+      </c>
+      <c r="E201">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" hidden="1">
+      <c r="B202" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="1" t="s">
+      <c r="D202" t="s">
+        <v>191</v>
+      </c>
+      <c r="E202">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" hidden="1">
+      <c r="A203" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D203" t="s">
+        <v>191</v>
+      </c>
+      <c r="E203">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" hidden="1">
+      <c r="B204" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="B194" s="2" t="s">
+      <c r="D204" t="s">
+        <v>191</v>
+      </c>
+      <c r="E204">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" hidden="1">
+      <c r="C205" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="C195" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" s="1" t="s">
+      <c r="D205" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="B197" s="2" t="s">
+      <c r="E205">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" hidden="1">
+      <c r="A206" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="D206" t="s">
+        <v>191</v>
+      </c>
+      <c r="E206">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" hidden="1">
+      <c r="B207" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D207" t="s">
+        <v>191</v>
+      </c>
+      <c r="E207">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E207" xr:uid="{3C75D4DC-26E2-0D4C-8573-26CF2820C251}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="?"/>
+        <filter val="4.1"/>
+        <filter val="4.2"/>
+        <filter val="4.3"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E207">
+      <sortCondition ref="E1:E207"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E207">
+    <sortCondition ref="D2:D207"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F72D62E-5C54-894B-9EC3-02DCA6ABEE4A}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>